<commit_message>
work on paper 1 matlab figures
</commit_message>
<xml_diff>
--- a/doc/Paper1/tab/tables.xlsx
+++ b/doc/Paper1/tab/tables.xlsx
@@ -14,8 +14,11 @@
   <sheets>
     <sheet name="Parameter Distributions" sheetId="1" r:id="rId1"/>
     <sheet name="PixDeltas" sheetId="2" r:id="rId2"/>
-    <sheet name="HarrisDeltas" sheetId="4" r:id="rId3"/>
-    <sheet name="Correlations" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId3"/>
+    <sheet name="HarrisDeltas" sheetId="4" r:id="rId4"/>
+    <sheet name="Correlations" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Minimum</t>
   </si>
@@ -126,18 +129,132 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Camera Parameter</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>focal length</t>
+  </si>
+  <si>
+    <t>principal point x</t>
+  </si>
+  <si>
+    <t>principal point y</t>
+  </si>
+  <si>
+    <t>k1</t>
+  </si>
+  <si>
+    <t>k2</t>
+  </si>
+  <si>
+    <t>k3</t>
+  </si>
+  <si>
+    <t>k4</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>Processing Parameter</t>
+  </si>
+  <si>
+    <t>Align Photos</t>
+  </si>
+  <si>
+    <t>Max tiepoints</t>
+  </si>
+  <si>
+    <t>Max keypoints</t>
+  </si>
+  <si>
+    <t>dense reconstruction</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>miscellaneous settings</t>
+  </si>
+  <si>
+    <t>Camera Position used</t>
+  </si>
+  <si>
+    <t>GCPs used</t>
+  </si>
+  <si>
+    <t>optimization</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Processing Start</t>
+  </si>
+  <si>
+    <t>Processing End</t>
+  </si>
+  <si>
+    <t>Pointcloud Name</t>
+  </si>
+  <si>
+    <t>high_aggressive</t>
+  </si>
+  <si>
+    <t>medium_aggressive</t>
+  </si>
+  <si>
+    <t>low_aggressive</t>
+  </si>
+  <si>
+    <t>lowest_aggressive</t>
+  </si>
+  <si>
+    <t>H:M:S</t>
+  </si>
+  <si>
+    <t>medium_disabled</t>
+  </si>
+  <si>
+    <t>Number of Points</t>
+  </si>
+  <si>
+    <t>ultrahigh_aggressive</t>
+  </si>
+  <si>
+    <t>sparse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -165,13 +282,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,7 +685,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="A2:K2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,8 +747,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <f>DEGREES(ATAN2(C3,D3/2))</f>
-        <v>11.460104538443192</v>
+        <f t="shared" ref="B3:B4" si="0">2*DEGREES(ATAN2(C3,D3/2))</f>
+        <v>22.920209076886383</v>
       </c>
       <c r="C3">
         <v>55</v>
@@ -663,8 +783,8 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <f>DEGREES(ATAN2(C4,D4/2))</f>
-        <v>28.971480746702643</v>
+        <f t="shared" si="0"/>
+        <v>57.942961493405285</v>
       </c>
       <c r="C4">
         <v>4.0999999999999996</v>
@@ -699,8 +819,8 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <f>DEGREES(ATAN2(C5,D5/2))</f>
-        <v>36.292629728479596</v>
+        <f>2*DEGREES(ATAN2(C5,D5/2))</f>
+        <v>72.585259456959193</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -735,8 +855,8 @@
         <v>3</v>
       </c>
       <c r="B6" s="2">
-        <f>DEGREES(ATAN2(C6,D6/2))</f>
-        <v>36.892196060562988</v>
+        <f t="shared" ref="B6:B7" si="1">2*DEGREES(ATAN2(C6,D6/2))</f>
+        <v>73.784392121125975</v>
       </c>
       <c r="C6">
         <v>4.1100000000000003</v>
@@ -771,8 +891,8 @@
         <v>4</v>
       </c>
       <c r="B7" s="2">
-        <f>DEGREES(ATAN2(C7,D7/2))</f>
-        <v>46.7704837517445</v>
+        <f t="shared" si="1"/>
+        <v>93.540967503489</v>
       </c>
       <c r="C7">
         <v>2.9</v>
@@ -812,9 +932,175 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="4">
+        <v>42739.245787037034</v>
+      </c>
+      <c r="C2" s="4">
+        <v>42739.26635416667</v>
+      </c>
+      <c r="D2" s="5">
+        <f>C2-B2</f>
+        <v>2.0567129635310266E-2</v>
+      </c>
+      <c r="E2">
+        <v>11594234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="4">
+        <v>42738.748657407406</v>
+      </c>
+      <c r="C3" s="4">
+        <v>42739.245173611111</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D9" si="0">C3-B3</f>
+        <v>0.49651620370423188</v>
+      </c>
+      <c r="E3">
+        <v>186313448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="4">
+        <v>42738.651805555557</v>
+      </c>
+      <c r="C4" s="4">
+        <v>42738.748506944445</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>9.6701388887595385E-2</v>
+      </c>
+      <c r="E4">
+        <v>46465218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="4">
+        <v>42738.630277777775</v>
+      </c>
+      <c r="C5" s="4">
+        <v>42738.651770833334</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1493055559403729E-2</v>
+      </c>
+      <c r="E5">
+        <v>11587504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="4">
+        <v>42738.62394675926</v>
+      </c>
+      <c r="C6" s="4">
+        <v>42738.630266203705</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>6.3194444446708076E-3</v>
+      </c>
+      <c r="E6">
+        <v>2886971</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="4">
+        <v>42738.621458333335</v>
+      </c>
+      <c r="C7" s="4">
+        <v>42738.62394675926</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>2.488425925548654E-3</v>
+      </c>
+      <c r="E7">
+        <v>716331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="4">
+        <v>42739.573796296296</v>
+      </c>
+      <c r="C9" s="4">
+        <v>42739.598807870374</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5011574078234844E-2</v>
+      </c>
+      <c r="E9">
+        <v>22214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -870,7 +1156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -971,4 +1257,163 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="A1:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add results to paper 1
</commit_message>
<xml_diff>
--- a/doc/Paper1/tab/tables.xlsx
+++ b/doc/Paper1/tab/tables.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
   <si>
     <t>Minimum</t>
   </si>
@@ -234,6 +234,48 @@
   </si>
   <si>
     <t>sparse</t>
+  </si>
+  <si>
+    <t>Processing CPU</t>
+  </si>
+  <si>
+    <t>Intel Xeon CPU E5-1603 v3 @ 2.80GHz 2.70GHz</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>32 GB</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Windows 7 Enterprise 64 bit</t>
+  </si>
+  <si>
+    <t>GeForce GTX 980</t>
+  </si>
+  <si>
+    <t>what type of hard drive</t>
+  </si>
+  <si>
+    <t>dense lowest</t>
+  </si>
+  <si>
+    <t>dense low</t>
+  </si>
+  <si>
+    <t>dense medium</t>
+  </si>
+  <si>
+    <t>dense high</t>
+  </si>
+  <si>
+    <t>dense ultrahigh</t>
   </si>
 </sst>
 </file>
@@ -282,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -292,6 +334,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,10 +978,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1136,122 @@
         <v>22214</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="5">
+        <v>2.5011574078234844E-2</v>
+      </c>
+      <c r="C18">
+        <v>22214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2.488425925548654E-3</v>
+      </c>
+      <c r="C19">
+        <v>716331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="5">
+        <v>6.3194444446708076E-3</v>
+      </c>
+      <c r="C20">
+        <v>2886971</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2.1493055559403729E-2</v>
+      </c>
+      <c r="C21">
+        <v>11587504</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="5">
+        <v>9.6701388887595385E-2</v>
+      </c>
+      <c r="C22">
+        <v>46465218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="5">
+        <v>0.49651620370423188</v>
+      </c>
+      <c r="C23">
+        <v>186313448</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A18:C23">
+    <sortCondition ref="C18:C23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
working on paper 1
almost to first draft
</commit_message>
<xml_diff>
--- a/doc/Paper1/tab/tables.xlsx
+++ b/doc/Paper1/tab/tables.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richie\Documents\GitHub\BlenderPythonTest\doc\Paper1\tab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="0" windowWidth="16365" windowHeight="13215" activeTab="2"/>
+    <workbookView xWindow="4980" yWindow="0" windowWidth="16365" windowHeight="13215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter Distributions" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="84">
   <si>
     <t>Minimum</t>
   </si>
@@ -276,6 +277,12 @@
   </si>
   <si>
     <t>dense ultrahigh</t>
+  </si>
+  <si>
+    <t>RMSE Mean</t>
+  </si>
+  <si>
+    <t>RMSE STD</t>
   </si>
 </sst>
 </file>
@@ -283,9 +290,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="173" formatCode="[h]:mm:ss;@"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="[h]:mm:ss;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -324,19 +331,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,10 +756,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -792,8 +800,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <f t="shared" ref="B3:B4" si="0">2*DEGREES(ATAN2(C3,D3/2))</f>
+      <c r="B3" s="3">
+        <f>2*DEGREES(ATAN2(C3,D3/2))</f>
         <v>22.920209076886383</v>
       </c>
       <c r="C3">
@@ -828,8 +836,8 @@
       <c r="A4">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
-        <f t="shared" si="0"/>
+      <c r="B4" s="3">
+        <f>2*DEGREES(ATAN2(C4,D4/2))</f>
         <v>57.942961493405285</v>
       </c>
       <c r="C4">
@@ -864,7 +872,7 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <f>2*DEGREES(ATAN2(C5,D5/2))</f>
         <v>72.585259456959193</v>
       </c>
@@ -900,8 +908,8 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="2">
-        <f t="shared" ref="B6:B7" si="1">2*DEGREES(ATAN2(C6,D6/2))</f>
+      <c r="B6" s="3">
+        <f>2*DEGREES(ATAN2(C6,D6/2))</f>
         <v>73.784392121125975</v>
       </c>
       <c r="C6">
@@ -936,8 +944,8 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="2">
-        <f t="shared" si="1"/>
+      <c r="B7" s="3">
+        <f>2*DEGREES(ATAN2(C7,D7/2))</f>
         <v>93.540967503489</v>
       </c>
       <c r="C7">
@@ -978,10 +986,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:B23"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1179,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>58</v>
       </c>
@@ -1181,8 +1189,14 @@
       <c r="C17" s="7" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -1192,8 +1206,18 @@
       <c r="C18">
         <v>22214</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" ref="D18:D23" si="1">INT(B18)*24+HOUR(B18)+ROUND(MINUTE(B18)/60,2)</f>
+        <v>0.6</v>
+      </c>
+      <c r="E18">
+        <v>-6.0000000000000002E-5</v>
+      </c>
+      <c r="F18">
+        <v>2.7899999999999999E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -1203,8 +1227,18 @@
       <c r="C19">
         <v>716331</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="E19">
+        <v>-6.6E-3</v>
+      </c>
+      <c r="F19">
+        <v>3.2300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -1214,8 +1248,18 @@
       <c r="C20">
         <v>2886971</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <f t="shared" si="1"/>
+        <v>0.15</v>
+      </c>
+      <c r="E20">
+        <v>-2E-3</v>
+      </c>
+      <c r="F20">
+        <v>1.54E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1225,8 +1269,18 @@
       <c r="C21">
         <v>11587504</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>-5.0000000000000001E-4</v>
+      </c>
+      <c r="F21">
+        <v>7.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -1236,8 +1290,18 @@
       <c r="C22">
         <v>46465218</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <f t="shared" si="1"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="E22">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="F22">
+        <v>4.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1246,6 +1310,16 @@
       </c>
       <c r="C23">
         <v>186313448</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="1"/>
+        <v>11.9</v>
+      </c>
+      <c r="E23">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="F23">
+        <v>2.5999999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>